<commit_message>
completed the test-plan for investment-account
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\rrc-polytech\semester-2\Intermidiate software development\Assignment-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA258353-9705-4DB9-B26C-6083DDC66CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E4480E-3E3E-4B97-89F3-165CF5083484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -266,22 +266,25 @@
     <t>service_charge set to 2.50</t>
   </si>
   <si>
-    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2024, 3, 25), management_fee = 2</t>
-  </si>
-  <si>
-    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2014, 3, 25), management_fee = 2</t>
-  </si>
-  <si>
-    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2024, 3, 25), management_fee = 'two'</t>
-  </si>
-  <si>
-    <t>account_number = 350, client_number = 350, balance = 350, date_created = InvestmentAccount.TEN_YEARS_AGO, management_fee = 2</t>
-  </si>
-  <si>
-    <t>Account Number: 350 Balance: $350.00 Date Created: 2014-03-25 Management Fee: Waived Account Type: Investment</t>
-  </si>
-  <si>
-    <t>Account Number: 350 Balance: $350.00 Date Created: 2024-03-25 Management Fee: $2.00 Account Type: Investment</t>
+    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2024, 5, 10), management_fee = 3</t>
+  </si>
+  <si>
+    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2024, 3, 25), management_fee = 'three'</t>
+  </si>
+  <si>
+    <t>account_number = 350, client_number = 350, balance = 350, date_created = InvestmentAccount.TEN_YEARS_AGO, management_fee = 3</t>
+  </si>
+  <si>
+    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2024, 3, 25), management_fee = 3</t>
+  </si>
+  <si>
+    <t>account_number = 350, client_number = 350, balance = 350, date_created = (2014, 3, 25), management_fee = 3</t>
+  </si>
+  <si>
+    <t>Account Number: 350 Balance: $350.00 Date Created: 2024-05-10 Management Fee: $3.00 Account Type: Investment</t>
+  </si>
+  <si>
+    <t>Account Number: 350 Balance: $350.00 Date Created: 2014-05-10 Management Fee: Waived Account Type: Investment</t>
   </si>
 </sst>
 </file>
@@ -1188,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,7 +1293,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>24</v>
@@ -1310,7 +1313,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>25</v>
@@ -1330,7 +1333,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>26</v>
@@ -1350,7 +1353,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>26</v>
@@ -1370,10 +1373,10 @@
         <v>22</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1390,7 +1393,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Minor edits in investment_account file
</commit_message>
<xml_diff>
--- a/tests/A02_pixell_test_plan_investment_account.xlsx
+++ b/tests/A02_pixell_test_plan_investment_account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\rrc-polytech\semester-2\Intermidiate software development\Assignment-1\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E4480E-3E3E-4B97-89F3-165CF5083484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5067BD91-F595-448F-9B84-B0A125038A13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
@@ -263,9 +263,6 @@
     <t>service_charge set to 0.50</t>
   </si>
   <si>
-    <t>service_charge set to 2.50</t>
-  </si>
-  <si>
     <t>account_number = 350, client_number = 350, balance = 350, date_created = (2024, 5, 10), management_fee = 3</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>Account Number: 350 Balance: $350.00 Date Created: 2014-05-10 Management Fee: Waived Account Type: Investment</t>
+  </si>
+  <si>
+    <t>service_charge set to 3.50</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="B1:G34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1273,7 +1273,7 @@
         <v>22</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>23</v>
@@ -1293,7 +1293,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>24</v>
@@ -1313,7 +1313,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>25</v>
@@ -1333,10 +1333,10 @@
         <v>22</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1353,10 +1353,10 @@
         <v>22</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1373,10 +1373,10 @@
         <v>22</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1393,10 +1393,10 @@
         <v>22</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>